<commit_message>
Aggiungo script per risultati per gruppo
</commit_message>
<xml_diff>
--- a/results/best_ksvm_for_each_category.xlsx
+++ b/results/best_ksvm_for_each_category.xlsx
@@ -14,11 +14,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>kfun</t>
+  </si>
+  <si>
+    <t>lambda</t>
+  </si>
+  <si>
+    <t>kparam</t>
+  </si>
   <si>
     <t>lr</t>
   </si>
   <si>
+    <t>index</t>
+  </si>
+  <si>
     <t>train</t>
   </si>
   <si>
@@ -41,6 +56,42 @@
   </si>
   <si>
     <t>rgb_cooccurrence_matrix</t>
+  </si>
+  <si>
+    <t>ksvm</t>
+  </si>
+  <si>
+    <t>rbf</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>0.002</t>
+  </si>
+  <si>
+    <t>0.003</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>ksvm_kfun=rbf_lambda_=0.3_kparam=0.001_lr=0.01__color_histogram</t>
+  </si>
+  <si>
+    <t>ksvm_kfun=rbf_lambda_=0.1_kparam=0.003_lr=0.003__cooccurrence_matrix</t>
+  </si>
+  <si>
+    <t>ksvm_kfun=rbf_lambda_=0.3_kparam=0.001_lr=0.01__deepfeatures</t>
+  </si>
+  <si>
+    <t>ksvm_kfun=rbf_lambda_=0.002_kparam=0.2_lr=0.03__edge_direction_histogram</t>
+  </si>
+  <si>
+    <t>ksvm_kfun=rbf_lambda_=0.003_kparam=0.1_lr=0.003__rgb_cooccurrence_matrix</t>
   </si>
 </sst>
 </file>
@@ -398,15 +449,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -417,74 +468,164 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2">
         <v>0.1</v>
       </c>
-      <c r="C2">
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2">
         <v>0.344279661016949</v>
       </c>
-      <c r="D2">
+      <c r="I2">
         <v>0.333333333333333</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3">
         <v>0.1</v>
       </c>
-      <c r="C3">
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3">
         <v>0.344279661016949</v>
       </c>
-      <c r="D3">
+      <c r="I3">
         <v>0.333333333333333</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4">
         <v>0.1</v>
       </c>
-      <c r="C4">
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4">
         <v>0.9242584745762711</v>
       </c>
-      <c r="D4">
+      <c r="I4">
         <v>0.9666666666666661</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5">
         <v>0.1</v>
       </c>
-      <c r="C5">
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5">
         <v>0.344279661016949</v>
       </c>
-      <c r="D5">
+      <c r="I5">
         <v>0.333333333333333</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6">
         <v>0.1</v>
       </c>
-      <c r="C6">
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6">
         <v>0.344279661016949</v>
       </c>
-      <c r="D6">
+      <c r="I6">
         <v>0.333333333333333</v>
       </c>
     </row>

</xml_diff>